<commit_message>
Removes schedule W from schedule export logic
</commit_message>
<xml_diff>
--- a/cypress/fixtures/grafik.xlsx
+++ b/cypress/fixtures/grafik.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="66">
   <si>
     <t xml:space="preserve">Grafik </t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>DN</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
   <si>
     <t>U</t>
@@ -1320,1067 +1317,1067 @@
         <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="S6" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y6" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AG6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AK6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AL6" s="1" t="s">
+      <c r="AM6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="I7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="S7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AF7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AG7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AI7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ7" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AK7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AL7" s="1" t="s">
+      <c r="AM7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="AM7" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="R8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="X8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Z8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AB8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AG8" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AJ8" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AK8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AL8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="AM8" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AK9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL9" s="1" t="s">
+      <c r="AM9" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="AM9" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="S10" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="W10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Z10" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AF10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AG10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="AL10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AM10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X11" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AD11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AG11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AJ11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AK11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AL11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AL11" s="1" t="s">
+      <c r="AM11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="AM11" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AK12" s="1" t="s">
+      <c r="AL12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AL12" s="1" t="s">
+      <c r="AM12" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="AM12" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AI13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL13" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="AM13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="S14" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="X14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="Y14" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AC14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AF14" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AG14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AJ14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AK14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AL14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AM14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:100" x14ac:dyDescent="0.25">
@@ -2687,1192 +2684,1192 @@
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="T16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="U16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="V16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="W16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG16" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AK16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL16" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="AM16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="W17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK17" s="1" t="s">
+      <c r="AL17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AL17" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="AM17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S18" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="V18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z18" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AF18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AG18" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AH18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AI18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AJ18" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AK18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AL18" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AM18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="S19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="V19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA19" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="X19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA19" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="AB19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AF19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AG19" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AH19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AI19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AJ19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK19" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="AL19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM19" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="AM19" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="O20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z20" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="AD20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N20" s="1" t="s">
+      <c r="AL20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="X20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AJ20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL20" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="AM20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>12</v>
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Z21" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AD21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AE21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AF21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AG21" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AJ21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AK21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AL21" s="1" t="s">
+      <c r="AM21" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="AM21" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>12</v>
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L22" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="W22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z22" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AE22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF22" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AG22" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AH22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AI22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AJ22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AL22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AM22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ23" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="S23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="T23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="U23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="W23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ23" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK23" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="AL23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AM23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>12</v>
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="S24" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Y24" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Z24" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AD24" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="AE24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AG24" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AH24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AI24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AJ24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AK24" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AL24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AM24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="V25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ25" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM25" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="V25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="X25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG25" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ25" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AL25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM25" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:100" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add param to specify month and year to loading schedule function
</commit_message>
<xml_diff>
--- a/cypress/fixtures/grafik.xlsx
+++ b/cypress/fixtures/grafik.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="70">
   <si>
     <t xml:space="preserve">Grafik </t>
   </si>
@@ -160,6 +160,15 @@
     <t>36</t>
   </si>
   <si>
+    <t>opiekunka 10</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
     <t>opiekunka 2</t>
   </si>
   <si>
@@ -181,9 +190,6 @@
     <t>248</t>
   </si>
   <si>
-    <t>96</t>
-  </si>
-  <si>
     <t>opiekunka 5</t>
   </si>
   <si>
@@ -215,12 +221,6 @@
   </si>
   <si>
     <t>184</t>
-  </si>
-  <si>
-    <t>opiekunka 10</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
 </sst>
 </file>
@@ -680,116 +680,134 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>31</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="J2">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="K2">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="N2">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="O2">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="P2">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="Q2">
         <v>10</v>
       </c>
-      <c r="L2">
-        <v>11</v>
-      </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
-      <c r="N2">
+      <c r="R2">
+        <v>11</v>
+      </c>
+      <c r="S2">
+        <v>12</v>
+      </c>
+      <c r="T2">
         <v>13</v>
       </c>
-      <c r="O2">
+      <c r="U2">
         <v>14</v>
       </c>
-      <c r="P2">
+      <c r="V2">
         <v>15</v>
       </c>
-      <c r="Q2">
+      <c r="W2">
         <v>16</v>
       </c>
-      <c r="R2">
+      <c r="X2">
         <v>17</v>
       </c>
-      <c r="S2">
+      <c r="Y2">
         <v>18</v>
       </c>
-      <c r="T2">
-        <v>19</v>
-      </c>
-      <c r="U2">
+      <c r="Z2">
+        <v>19</v>
+      </c>
+      <c r="AA2">
         <v>20</v>
       </c>
-      <c r="V2">
+      <c r="AB2">
         <v>21</v>
       </c>
-      <c r="W2">
+      <c r="AC2">
         <v>22</v>
       </c>
-      <c r="X2">
+      <c r="AD2">
         <v>23</v>
       </c>
-      <c r="Y2">
+      <c r="AE2">
         <v>24</v>
       </c>
-      <c r="Z2">
+      <c r="AF2">
         <v>25</v>
       </c>
-      <c r="AA2">
+      <c r="AG2">
         <v>26</v>
       </c>
-      <c r="AB2">
+      <c r="AH2">
         <v>27</v>
       </c>
-      <c r="AC2">
+      <c r="AI2">
         <v>28</v>
       </c>
-      <c r="AD2">
+      <c r="AJ2">
         <v>29</v>
       </c>
-      <c r="AE2">
+      <c r="AK2">
         <v>30</v>
       </c>
-      <c r="AF2">
+      <c r="AL2">
         <v>1</v>
       </c>
-      <c r="AG2">
+      <c r="AM2">
         <v>2</v>
       </c>
-      <c r="AH2">
+      <c r="AN2">
         <v>3</v>
       </c>
-      <c r="AI2">
+      <c r="AO2">
         <v>4</v>
       </c>
-      <c r="AJ2">
-        <v>5</v>
-      </c>
-      <c r="AK2">
+      <c r="AP2">
+        <v>5</v>
+      </c>
+      <c r="AQ2">
         <v>6</v>
       </c>
     </row>
@@ -1095,27 +1113,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>24</v>
@@ -1190,25 +1208,43 @@
         <v>24</v>
       </c>
       <c r="AF4">
+        <v>24</v>
+      </c>
+      <c r="AG4">
+        <v>24</v>
+      </c>
+      <c r="AH4">
+        <v>24</v>
+      </c>
+      <c r="AI4">
+        <v>24</v>
+      </c>
+      <c r="AJ4">
+        <v>24</v>
+      </c>
+      <c r="AK4">
+        <v>24</v>
+      </c>
+      <c r="AL4">
         <v>0</v>
       </c>
-      <c r="AG4">
+      <c r="AM4">
         <v>0</v>
       </c>
-      <c r="AH4">
+      <c r="AN4">
         <v>0</v>
       </c>
-      <c r="AI4">
+      <c r="AO4">
         <v>0</v>
       </c>
-      <c r="AJ4">
+      <c r="AP4">
         <v>0</v>
       </c>
-      <c r="AK4">
+      <c r="AQ4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1321,206 +1357,242 @@
         <v>5</v>
       </c>
       <c r="AL5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR5" t="s">
         <v>7</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AS5" t="s">
         <v>8</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AT5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N6" s="2" t="s">
+      <c r="Q6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="4" t="s">
+      <c r="U6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="X6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="W6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="X6" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="Y6" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AB6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC6" s="3" t="s">
+      <c r="AH6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AD6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ6" s="3" t="s">
+      <c r="AJ6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AK6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AL6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AM6" s="4" t="s">
+      <c r="AS6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AN6" s="4" t="s">
+      <c r="AT6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="3" t="s">
+      <c r="M7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="T7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="V7" s="3" t="s">
+      <c r="V7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="X7" s="4" t="s">
         <v>19</v>
@@ -1529,142 +1601,160 @@
         <v>19</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AC7" s="3" t="s">
+      <c r="AI7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AD7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE7" s="4" t="s">
+      <c r="AJ7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AF7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK7" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="AL7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AM7" s="4" t="s">
+      <c r="AS7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AN7" s="4" t="s">
+      <c r="AT7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="N8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="5" t="s">
+      <c r="P8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2" t="s">
+      <c r="R8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="4" t="s">
+      <c r="U8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="T8" s="4" t="s">
+      <c r="X8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="U8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="X8" s="4" t="s">
+      <c r="AA8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD8" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="AE8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1674,100 +1764,118 @@
       <c r="AG8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AH8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ8" s="3" t="s">
-        <v>5</v>
+      <c r="AH8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="AK8" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="AL8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AM8" s="4" t="s">
+      <c r="AS8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AN8" s="4" t="s">
+      <c r="AT8" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>19</v>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="P9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="Q9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="T9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="W9" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="X9" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Y9" s="4" t="s">
         <v>5</v>
@@ -1775,50 +1883,68 @@
       <c r="Z9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AA9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>11</v>
+      <c r="AA9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="AF9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AG9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK9" s="4" t="s">
-        <v>5</v>
+      <c r="AG9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="AL9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AM9" s="4" t="s">
+      <c r="AS9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AN9" s="4" t="s">
+      <c r="AT9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1834,135 +1960,153 @@
       <c r="E10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="5" t="s">
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="P10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S10" s="4" t="s">
+      <c r="W10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="W10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="X10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="Z10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AA10" s="4" t="s">
+      <c r="AA10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AB10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AH10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="AD10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE10" s="4" t="s">
+      <c r="AJ10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AF10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK10" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="AL10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AM10" s="4" t="s">
+      <c r="AS10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AN10" s="4" t="s">
+      <c r="AT10" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -1971,147 +2115,165 @@
       <c r="J11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="3" t="s">
+      <c r="M11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="X11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z11" s="4" t="s">
+      <c r="S11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AA11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC11" s="3" t="s">
+      <c r="AG11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AD11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ11" s="3" t="s">
-        <v>5</v>
+      <c r="AJ11" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AK11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AL11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AM11" s="4" t="s">
+      <c r="AS11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AN11" s="4" t="s">
+      <c r="AT11" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>11</v>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O12" s="3" t="s">
+      <c r="M12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R12" s="1" t="s">
@@ -2120,311 +2282,365 @@
       <c r="S12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC12" s="3" t="s">
+      <c r="T12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AD12" s="4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AE12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AF12" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="AG12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AH12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ12" s="3" t="s">
-        <v>5</v>
+      <c r="AH12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ12" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AK12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AL12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AM12" s="4" t="s">
+      <c r="AS12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AN12" s="4" t="s">
+      <c r="AT12" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>5</v>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="M13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>5</v>
+      <c r="T13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="X13" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AB13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ13" s="3" t="s">
-        <v>5</v>
+      <c r="AH13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ13" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="AK13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AL13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AM13" s="4" t="s">
+      <c r="AS13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AN13" s="4" t="s">
+      <c r="AT13" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="4" t="s">
+      <c r="O14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M14" s="4" t="s">
+      <c r="Q14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="R14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="T14" s="4" t="s">
+      <c r="T14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="U14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="V14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="W14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="X14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y14" s="4" t="s">
+      <c r="AA14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Z14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA14" s="4" t="s">
+      <c r="AF14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG14" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AB14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC14" s="3" t="s">
+      <c r="AH14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AD14" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
-        <v>5</v>
+      <c r="AJ14" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AK14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AL14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AM14" s="4" t="s">
+      <c r="AS14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AN14" s="4" t="s">
+      <c r="AT14" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2730,56 +2946,56 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>11</v>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O16" s="3" t="s">
+      <c r="M16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R16" s="1" t="s">
@@ -2788,136 +3004,154 @@
       <c r="S16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T16" s="4" t="s">
+      <c r="T16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="U16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="X16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC16" s="3" t="s">
+      <c r="AA16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="AD16" s="4" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AE16" s="4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="AF16" s="4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="AG16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AH16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ16" s="3" t="s">
-        <v>5</v>
+      <c r="AH16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ16" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="AK16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="AL16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR16" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AM16" s="4" t="s">
+      <c r="AS16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AN16" s="4" t="s">
+      <c r="AT16" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="S17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V17" s="3" t="s">
-        <v>33</v>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="W17" s="6" t="s">
         <v>33</v>
@@ -2931,13 +3165,13 @@
       <c r="Z17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AA17" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC17" s="3" t="s">
+      <c r="AA17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC17" s="6" t="s">
         <v>33</v>
       </c>
       <c r="AD17" s="6" t="s">
@@ -2946,423 +3180,495 @@
       <c r="AE17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AF17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK17" s="4" t="s">
-        <v>5</v>
+      <c r="AF17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK17" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="AL17" s="4" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="AM17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AS17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AN17" s="4" t="s">
+      <c r="AT17" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB18" s="2" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AS18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT18" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AC18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE18" s="4" t="s">
+      <c r="AI19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AF18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL18" s="4" t="s">
+      <c r="AL19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="AM18" s="4" t="s">
+      <c r="AS19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AN18" s="4" t="s">
-        <v>53</v>
+      <c r="AT19" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="T19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="V19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="W19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="X19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AC19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM19" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN19" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="3" t="s">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" t="s">
         <v>5</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC20" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="T20" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V20" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="X20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AM20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="AN20" s="4" t="s">
-        <v>22</v>
+      <c r="AT20" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I21" s="4" t="s">
@@ -3371,583 +3677,673 @@
       <c r="J21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q21" s="4" t="s">
-        <v>5</v>
+        <v>60</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="R21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="X21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AT21" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="S21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="T21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="V21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="W21" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="X21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z21" s="4" t="s">
+      <c r="Y22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AA21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB21" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL21" s="4" t="s">
+      <c r="AG22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AM21" s="4" t="s">
+      <c r="AS22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AN21" s="4" t="s">
+      <c r="AT22" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="3" t="s">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N22" s="2" t="s">
+      <c r="O23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="T23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q22" s="4" t="s">
+      <c r="U23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="W22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN22" s="4" t="s">
+      <c r="X23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT23" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="S23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="W23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="X23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE23" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL23" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AM23" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AN23" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="R24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="S24" s="4" t="s">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="W24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="X24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK24" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT24" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y25" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="U24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="X24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL24" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM24" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN24" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="Z25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR25" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="W25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="X25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB25" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE25" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AM25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN25" s="4" t="s">
+      <c r="AS25" s="4" t="s">
         <v>69</v>
+      </c>
+      <c r="AT25" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:100" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove code duplication from nextMonthKey and prevMonthKey
</commit_message>
<xml_diff>
--- a/cypress/fixtures/grafik.xlsx
+++ b/cypress/fixtures/grafik.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="71">
   <si>
     <t xml:space="preserve">Grafik </t>
   </si>
@@ -58,147 +58,156 @@
     <t>DN</t>
   </si>
   <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>pielęgniarka 2</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>pielęgniarka 3</t>
+  </si>
+  <si>
+    <t>264</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>pielęgniarka 4</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>pielęgniarka 5</t>
+  </si>
+  <si>
+    <t>-16</t>
+  </si>
+  <si>
+    <t>pielęgniarka 6</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>pielęgniarka 7</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>pielęgniarka 8</t>
+  </si>
+  <si>
+    <t>196</t>
+  </si>
+  <si>
+    <t>pielęgniarka 9</t>
+  </si>
+  <si>
     <t>120</t>
   </si>
   <si>
-    <t>152</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>pielęgniarka 2</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>PN</t>
-  </si>
-  <si>
     <t>216</t>
   </si>
   <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>opiekunka 1</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>opiekunka 2</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>opiekunka 3</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>opiekunka 4</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>opiekunka 5</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
     <t>64</t>
   </si>
   <si>
-    <t>pielęgniarka 3</t>
-  </si>
-  <si>
-    <t>252</t>
-  </si>
-  <si>
-    <t>132</t>
-  </si>
-  <si>
-    <t>pielęgniarka 4</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>pielęgniarka 5</t>
-  </si>
-  <si>
-    <t>-24</t>
-  </si>
-  <si>
-    <t>pielęgniarka 6</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>pielęgniarka 7</t>
-  </si>
-  <si>
-    <t>72</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>pielęgniarka 8</t>
-  </si>
-  <si>
-    <t>196</t>
-  </si>
-  <si>
-    <t>pielęgniarka 9</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>opiekunka 1</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>opiekunka 2</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>opiekunka 3</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>opiekunka 4</t>
-  </si>
-  <si>
-    <t>248</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>opiekunka 5</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>opiekunka 6</t>
   </si>
   <si>
+    <t>56</t>
+  </si>
+  <si>
     <t>opiekunka 7</t>
   </si>
   <si>
-    <t>88</t>
-  </si>
-  <si>
     <t>168</t>
   </si>
   <si>
@@ -211,16 +220,10 @@
     <t>opiekunka 9</t>
   </si>
   <si>
-    <t>136</t>
-  </si>
-  <si>
     <t>184</t>
   </si>
   <si>
     <t>opiekunka 10</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
 </sst>
 </file>
@@ -1655,18 +1658,18 @@
         <v>5</v>
       </c>
       <c r="AR7" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AS7" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1798,15 +1801,15 @@
         <v>15</v>
       </c>
       <c r="AS8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AT8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1935,7 +1938,7 @@
         <v>5</v>
       </c>
       <c r="AR9" s="4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="AS9" s="4" t="s">
         <v>28</v>
@@ -2075,10 +2078,10 @@
         <v>5</v>
       </c>
       <c r="AR10" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AS10" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AT10" s="4" t="s">
         <v>31</v>
@@ -2355,18 +2358,18 @@
         <v>5</v>
       </c>
       <c r="AR12" s="4" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="AS12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="AT12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
@@ -2495,10 +2498,10 @@
         <v>5</v>
       </c>
       <c r="AR13" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AS13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AT13" s="4" t="s">
         <v>36</v>
@@ -2506,7 +2509,7 @@
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -2635,10 +2638,10 @@
         <v>5</v>
       </c>
       <c r="AR14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS14" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="AS14" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="AT14" s="4" t="s">
         <v>44</v>
@@ -3217,10 +3220,10 @@
         <v>5</v>
       </c>
       <c r="AR17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS17" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="AS17" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="AT17" s="4" t="s">
         <v>51</v>
@@ -3357,18 +3360,18 @@
         <v>5</v>
       </c>
       <c r="AR18" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="AS18" s="4" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="AT18" s="4" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
@@ -3497,18 +3500,18 @@
         <v>5</v>
       </c>
       <c r="AR19" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AS19" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AT19" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -3553,7 +3556,7 @@
         <v>12</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q20" s="5" t="s">
         <v>19</v>
@@ -3637,18 +3640,18 @@
         <v>5</v>
       </c>
       <c r="AR20" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AS20" s="4" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="AT20" s="4" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
@@ -3777,18 +3780,18 @@
         <v>5</v>
       </c>
       <c r="AR21" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="AS21" s="4" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="AT21" s="4" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -3917,18 +3920,18 @@
         <v>5</v>
       </c>
       <c r="AR22" s="4" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="AS22" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AT22" s="4" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -4057,18 +4060,18 @@
         <v>5</v>
       </c>
       <c r="AR23" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AS23" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="AT23" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -4122,7 +4125,7 @@
         <v>19</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T24" s="2" t="s">
         <v>5</v>
@@ -4197,18 +4200,18 @@
         <v>5</v>
       </c>
       <c r="AR24" s="4" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="AS24" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AT24" s="4" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -4337,13 +4340,13 @@
         <v>5</v>
       </c>
       <c r="AR25" s="4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="AS25" s="4" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="AT25" s="4" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:100" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Displaying error page test
</commit_message>
<xml_diff>
--- a/cypress/fixtures/grafik.xlsx
+++ b/cypress/fixtures/grafik.xlsx
@@ -40,81 +40,84 @@
     <t>Pielęgniarka 1</t>
   </si>
   <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 2</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>DN</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>164</t>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 3</t>
+  </si>
+  <si>
+    <t>264</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 4</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 5</t>
+  </si>
+  <si>
+    <t>-16</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 6</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>84</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>Pielęgniarka 2</t>
-  </si>
-  <si>
-    <t>PN</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 3</t>
-  </si>
-  <si>
-    <t>264</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 4</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 5</t>
-  </si>
-  <si>
-    <t>-16</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 6</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
     <t>Pielęgniarka 7</t>
   </si>
   <si>
@@ -215,9 +218,6 @@
   </si>
   <si>
     <t>Opiekunka 10</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
 </sst>
 </file>
@@ -252,11 +252,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="01c8dfff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="01ff8a00"/>
       </patternFill>
     </fill>
@@ -268,6 +263,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="01fac090"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="01c8dfff"/>
       </patternFill>
     </fill>
     <fill>
@@ -1317,178 +1317,178 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>10</v>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="O6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="AH6" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>11</v>
+      <c r="V7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z7" s="3" t="s">
         <v>6</v>
@@ -1497,16 +1497,16 @@
         <v>6</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="AD7" s="7" t="s">
+      <c r="AD7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF7" s="3" t="s">
         <v>19</v>
@@ -1522,98 +1522,98 @@
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>10</v>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF8" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF8" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="AG8" s="3" t="s">
         <v>23</v>
@@ -1626,53 +1626,53 @@
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>10</v>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>9</v>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="7" t="s">
+      <c r="O9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>6</v>
@@ -1684,16 +1684,16 @@
         <v>6</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y9" s="3" t="s">
         <v>6</v>
@@ -1701,23 +1701,23 @@
       <c r="Z9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>10</v>
+      <c r="AA9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AG9" s="3" t="s">
         <v>26</v>
@@ -1730,7 +1730,7 @@
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1743,15 +1743,15 @@
         <v>6</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="H10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J10" s="3" t="s">
@@ -1760,7 +1760,7 @@
       <c r="K10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1769,11 +1769,11 @@
       <c r="N10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>13</v>
+      <c r="O10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>6</v>
@@ -1782,7 +1782,7 @@
         <v>6</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>6</v>
@@ -1790,31 +1790,31 @@
       <c r="U10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V10" s="6" t="s">
+      <c r="V10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD10" s="7" t="s">
+      <c r="AD10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="AE10" s="3" t="s">
@@ -1834,56 +1834,56 @@
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>10</v>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>31</v>
@@ -1897,8 +1897,8 @@
       <c r="V11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="W11" s="7" t="s">
-        <v>9</v>
+      <c r="W11" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>6</v>
@@ -1907,19 +1907,19 @@
         <v>6</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD11" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE11" s="3" t="s">
         <v>6</v>
@@ -1931,77 +1931,77 @@
         <v>33</v>
       </c>
       <c r="AH11" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>10</v>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X12" s="3" t="s">
@@ -2011,19 +2011,19 @@
         <v>6</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AA12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD12" s="7" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE12" s="3" t="s">
         <v>6</v>
@@ -2035,99 +2035,99 @@
         <v>33</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="N13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="AB13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD13" s="7" t="s">
-        <v>11</v>
+      <c r="AC13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE13" s="3" t="s">
         <v>6</v>
@@ -2136,114 +2136,114 @@
         <v>19</v>
       </c>
       <c r="AG13" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH13" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>11</v>
+      <c r="O14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W14" s="7" t="s">
+      <c r="V14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="7" t="s">
-        <v>9</v>
+      <c r="AC14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG14" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH14" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:100" x14ac:dyDescent="0.25">
@@ -2550,82 +2550,82 @@
     </row>
     <row r="16" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="U16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W16" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="X16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AA16" s="3" t="s">
         <v>6</v>
@@ -2633,48 +2633,48 @@
       <c r="AB16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD16" s="7" t="s">
-        <v>9</v>
+      <c r="AC16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD16" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AF16" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AG16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AH16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I17" s="8" t="s">
@@ -2747,24 +2747,24 @@
         <v>31</v>
       </c>
       <c r="AF17" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AG17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="AH17" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>6</v>
@@ -2772,65 +2772,65 @@
       <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W18" s="5" t="s">
-        <v>10</v>
+      <c r="F18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z18" s="3" t="s">
         <v>6</v>
@@ -2839,102 +2839,102 @@
         <v>6</v>
       </c>
       <c r="AB18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD18" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="AC18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AH18" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="V19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W19" s="7" t="s">
+      <c r="X19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X19" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="Y19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z19" s="3" t="s">
         <v>6</v>
@@ -2943,146 +2943,146 @@
         <v>6</v>
       </c>
       <c r="AB19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD19" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="AC19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AF19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AG19" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AH19" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P20" s="7" t="s">
+      <c r="Z20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE20" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE20" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="AF20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AG20" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AH20" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>6</v>
@@ -3090,53 +3090,53 @@
       <c r="G21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="H21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W21" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="V21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>6</v>
@@ -3145,19 +3145,19 @@
         <v>6</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD21" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="AC21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE21" s="3" t="s">
         <v>6</v>
@@ -3166,111 +3166,111 @@
         <v>19</v>
       </c>
       <c r="AG21" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH21" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>9</v>
+        <v>62</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="7" t="s">
+      <c r="H22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="X22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE22" s="5" t="s">
-        <v>10</v>
+      <c r="S22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE22" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF22" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AG22" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AH22" s="3" t="s">
         <v>21</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>31</v>
@@ -3371,114 +3371,114 @@
         <v>31</v>
       </c>
       <c r="AF23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AG23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AH23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>9</v>
+        <v>66</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>9</v>
+      <c r="H24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P24" s="7" t="s">
+      <c r="O24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE24" s="5" t="s">
-        <v>10</v>
+      <c r="AA24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE24" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF24" s="3" t="s">
         <v>24</v>
       </c>
       <c r="AG24" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AH24" s="3" t="s">
         <v>32</v>
@@ -3486,52 +3486,52 @@
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="Q25" s="8" t="s">
         <v>31</v>
@@ -3579,13 +3579,13 @@
         <v>31</v>
       </c>
       <c r="AF25" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG25" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH25" s="3" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:100" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Task 348 Enable undo on corrupted schedule page (#265)
</commit_message>
<xml_diff>
--- a/cypress/fixtures/grafik.xlsx
+++ b/cypress/fixtures/grafik.xlsx
@@ -40,81 +40,84 @@
     <t>Pielęgniarka 1</t>
   </si>
   <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 2</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>DN</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>164</t>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 3</t>
+  </si>
+  <si>
+    <t>264</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 4</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 5</t>
+  </si>
+  <si>
+    <t>-16</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 6</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>84</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>Pielęgniarka 2</t>
-  </si>
-  <si>
-    <t>PN</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 3</t>
-  </si>
-  <si>
-    <t>264</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 4</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 5</t>
-  </si>
-  <si>
-    <t>-16</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 6</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
     <t>Pielęgniarka 7</t>
   </si>
   <si>
@@ -215,9 +218,6 @@
   </si>
   <si>
     <t>Opiekunka 10</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
 </sst>
 </file>
@@ -252,11 +252,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="01c8dfff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="01ff8a00"/>
       </patternFill>
     </fill>
@@ -268,6 +263,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="01fac090"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="01c8dfff"/>
       </patternFill>
     </fill>
     <fill>
@@ -1317,178 +1317,178 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>10</v>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="O6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="AH6" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>11</v>
+      <c r="V7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z7" s="3" t="s">
         <v>6</v>
@@ -1497,16 +1497,16 @@
         <v>6</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="AD7" s="7" t="s">
+      <c r="AD7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF7" s="3" t="s">
         <v>19</v>
@@ -1522,98 +1522,98 @@
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>10</v>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF8" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF8" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="AG8" s="3" t="s">
         <v>23</v>
@@ -1626,53 +1626,53 @@
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>10</v>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>9</v>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="7" t="s">
+      <c r="O9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>6</v>
@@ -1684,16 +1684,16 @@
         <v>6</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y9" s="3" t="s">
         <v>6</v>
@@ -1701,23 +1701,23 @@
       <c r="Z9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>10</v>
+      <c r="AA9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AG9" s="3" t="s">
         <v>26</v>
@@ -1730,7 +1730,7 @@
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1743,15 +1743,15 @@
         <v>6</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="H10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J10" s="3" t="s">
@@ -1760,7 +1760,7 @@
       <c r="K10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1769,11 +1769,11 @@
       <c r="N10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>13</v>
+      <c r="O10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>6</v>
@@ -1782,7 +1782,7 @@
         <v>6</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>6</v>
@@ -1790,31 +1790,31 @@
       <c r="U10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V10" s="6" t="s">
+      <c r="V10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD10" s="7" t="s">
+      <c r="AD10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="AE10" s="3" t="s">
@@ -1834,56 +1834,56 @@
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>10</v>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>31</v>
@@ -1897,8 +1897,8 @@
       <c r="V11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="W11" s="7" t="s">
-        <v>9</v>
+      <c r="W11" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>6</v>
@@ -1907,19 +1907,19 @@
         <v>6</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD11" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE11" s="3" t="s">
         <v>6</v>
@@ -1931,77 +1931,77 @@
         <v>33</v>
       </c>
       <c r="AH11" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>10</v>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X12" s="3" t="s">
@@ -2011,19 +2011,19 @@
         <v>6</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AA12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD12" s="7" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE12" s="3" t="s">
         <v>6</v>
@@ -2035,99 +2035,99 @@
         <v>33</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="N13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="AB13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD13" s="7" t="s">
-        <v>11</v>
+      <c r="AC13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE13" s="3" t="s">
         <v>6</v>
@@ -2136,114 +2136,114 @@
         <v>19</v>
       </c>
       <c r="AG13" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH13" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>11</v>
+      <c r="O14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W14" s="7" t="s">
+      <c r="V14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="7" t="s">
-        <v>9</v>
+      <c r="AC14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG14" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH14" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:100" x14ac:dyDescent="0.25">
@@ -2550,82 +2550,82 @@
     </row>
     <row r="16" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="U16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W16" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="X16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AA16" s="3" t="s">
         <v>6</v>
@@ -2633,48 +2633,48 @@
       <c r="AB16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD16" s="7" t="s">
-        <v>9</v>
+      <c r="AC16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD16" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AF16" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AG16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AH16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I17" s="8" t="s">
@@ -2747,24 +2747,24 @@
         <v>31</v>
       </c>
       <c r="AF17" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AG17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="AH17" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>6</v>
@@ -2772,65 +2772,65 @@
       <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W18" s="5" t="s">
-        <v>10</v>
+      <c r="F18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z18" s="3" t="s">
         <v>6</v>
@@ -2839,102 +2839,102 @@
         <v>6</v>
       </c>
       <c r="AB18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD18" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="AC18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AH18" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="V19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W19" s="7" t="s">
+      <c r="X19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X19" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="Y19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z19" s="3" t="s">
         <v>6</v>
@@ -2943,146 +2943,146 @@
         <v>6</v>
       </c>
       <c r="AB19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD19" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="AC19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AF19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AG19" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AH19" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P20" s="7" t="s">
+      <c r="Z20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE20" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE20" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="AF20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AG20" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AH20" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>6</v>
@@ -3090,53 +3090,53 @@
       <c r="G21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="H21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W21" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="V21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>6</v>
@@ -3145,19 +3145,19 @@
         <v>6</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD21" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="AC21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE21" s="3" t="s">
         <v>6</v>
@@ -3166,111 +3166,111 @@
         <v>19</v>
       </c>
       <c r="AG21" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH21" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>9</v>
+        <v>62</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="7" t="s">
+      <c r="H22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="X22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE22" s="5" t="s">
-        <v>10</v>
+      <c r="S22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE22" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF22" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AG22" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AH22" s="3" t="s">
         <v>21</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>31</v>
@@ -3371,114 +3371,114 @@
         <v>31</v>
       </c>
       <c r="AF23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AG23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AH23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>9</v>
+        <v>66</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>9</v>
+      <c r="H24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P24" s="7" t="s">
+      <c r="O24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE24" s="5" t="s">
-        <v>10</v>
+      <c r="AA24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE24" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF24" s="3" t="s">
         <v>24</v>
       </c>
       <c r="AG24" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AH24" s="3" t="s">
         <v>32</v>
@@ -3486,52 +3486,52 @@
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="Q25" s="8" t="s">
         <v>31</v>
@@ -3579,13 +3579,13 @@
         <v>31</v>
       </c>
       <c r="AF25" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG25" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH25" s="3" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:100" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
getting rid of warnings
</commit_message>
<xml_diff>
--- a/cypress/fixtures/grafik.xlsx
+++ b/cypress/fixtures/grafik.xlsx
@@ -40,81 +40,84 @@
     <t>Pielęgniarka 1</t>
   </si>
   <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 2</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>DN</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>164</t>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 3</t>
+  </si>
+  <si>
+    <t>264</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 4</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 5</t>
+  </si>
+  <si>
+    <t>-16</t>
+  </si>
+  <si>
+    <t>Pielęgniarka 6</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>84</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>Pielęgniarka 2</t>
-  </si>
-  <si>
-    <t>PN</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 3</t>
-  </si>
-  <si>
-    <t>264</t>
-  </si>
-  <si>
-    <t>136</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 4</t>
-  </si>
-  <si>
-    <t>144</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 5</t>
-  </si>
-  <si>
-    <t>-16</t>
-  </si>
-  <si>
-    <t>Pielęgniarka 6</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
     <t>Pielęgniarka 7</t>
   </si>
   <si>
@@ -215,9 +218,6 @@
   </si>
   <si>
     <t>Opiekunka 10</t>
-  </si>
-  <si>
-    <t>24</t>
   </si>
 </sst>
 </file>
@@ -252,11 +252,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="01c8dfff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="01ff8a00"/>
       </patternFill>
     </fill>
@@ -268,6 +263,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="01fac090"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="01c8dfff"/>
       </patternFill>
     </fill>
     <fill>
@@ -1317,178 +1317,178 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>10</v>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="O6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="3" t="s">
+      <c r="AB6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="V6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AG6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AG6" s="3" t="s">
+      <c r="AH6" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="AH6" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>11</v>
+      <c r="V7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z7" s="3" t="s">
         <v>6</v>
@@ -1497,16 +1497,16 @@
         <v>6</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="AD7" s="7" t="s">
+      <c r="AD7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF7" s="3" t="s">
         <v>19</v>
@@ -1522,98 +1522,98 @@
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>10</v>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF8" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF8" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="AG8" s="3" t="s">
         <v>23</v>
@@ -1626,53 +1626,53 @@
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>10</v>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>9</v>
+      <c r="H9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P9" s="7" t="s">
+      <c r="O9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>6</v>
@@ -1684,16 +1684,16 @@
         <v>6</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y9" s="3" t="s">
         <v>6</v>
@@ -1701,23 +1701,23 @@
       <c r="Z9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>10</v>
+      <c r="AA9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AG9" s="3" t="s">
         <v>26</v>
@@ -1730,7 +1730,7 @@
       <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1743,15 +1743,15 @@
         <v>6</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="H10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J10" s="3" t="s">
@@ -1760,7 +1760,7 @@
       <c r="K10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1769,11 +1769,11 @@
       <c r="N10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>13</v>
+      <c r="O10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>6</v>
@@ -1782,7 +1782,7 @@
         <v>6</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T10" s="3" t="s">
         <v>6</v>
@@ -1790,31 +1790,31 @@
       <c r="U10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V10" s="6" t="s">
+      <c r="V10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="X10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD10" s="7" t="s">
+      <c r="AD10" s="6" t="s">
         <v>6</v>
       </c>
       <c r="AE10" s="3" t="s">
@@ -1834,56 +1834,56 @@
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R11" s="5" t="s">
-        <v>10</v>
+      <c r="B11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>31</v>
@@ -1897,8 +1897,8 @@
       <c r="V11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="W11" s="7" t="s">
-        <v>9</v>
+      <c r="W11" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>6</v>
@@ -1907,19 +1907,19 @@
         <v>6</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD11" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD11" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE11" s="3" t="s">
         <v>6</v>
@@ -1931,77 +1931,77 @@
         <v>33</v>
       </c>
       <c r="AH11" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>10</v>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X12" s="3" t="s">
@@ -2011,19 +2011,19 @@
         <v>6</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AA12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD12" s="7" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="AC12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD12" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE12" s="3" t="s">
         <v>6</v>
@@ -2035,99 +2035,99 @@
         <v>33</v>
       </c>
       <c r="AH12" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="N13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="S13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="T13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA13" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="AB13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD13" s="7" t="s">
-        <v>11</v>
+      <c r="AC13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD13" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE13" s="3" t="s">
         <v>6</v>
@@ -2136,114 +2136,114 @@
         <v>19</v>
       </c>
       <c r="AG13" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH13" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="L14" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P14" s="7" t="s">
-        <v>11</v>
+      <c r="O14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W14" s="7" t="s">
+      <c r="V14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Z14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AB14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="7" t="s">
-        <v>9</v>
+      <c r="AC14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD14" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AG14" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH14" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" ht="18" customHeight="1" spans="1:100" x14ac:dyDescent="0.25">
@@ -2550,82 +2550,82 @@
     </row>
     <row r="16" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="U16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W16" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W16" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="X16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="Y16" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AA16" s="3" t="s">
         <v>6</v>
@@ -2633,48 +2633,48 @@
       <c r="AB16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AC16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="AD16" s="7" t="s">
-        <v>9</v>
+      <c r="AC16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD16" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE16" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AF16" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AG16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AH16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="I17" s="8" t="s">
@@ -2747,24 +2747,24 @@
         <v>31</v>
       </c>
       <c r="AF17" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AG17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="AH17" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>6</v>
@@ -2772,65 +2772,65 @@
       <c r="E18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W18" s="5" t="s">
-        <v>10</v>
+      <c r="F18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z18" s="3" t="s">
         <v>6</v>
@@ -2839,102 +2839,102 @@
         <v>6</v>
       </c>
       <c r="AB18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD18" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="AC18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD18" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AH18" s="3" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="V19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="S19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U19" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="V19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W19" s="7" t="s">
+      <c r="X19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="X19" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="Y19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="Z19" s="3" t="s">
         <v>6</v>
@@ -2943,146 +2943,146 @@
         <v>6</v>
       </c>
       <c r="AB19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD19" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="AC19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD19" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="AE19" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="AF19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AG19" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AH19" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>9</v>
+        <v>56</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P20" s="7" t="s">
+      <c r="Z20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE20" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="Q20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="R20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="S20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T20" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="U20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V20" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="X20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC20" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD20" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE20" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="AF20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="AG20" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AH20" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>6</v>
@@ -3090,53 +3090,53 @@
       <c r="G21" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="H21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="T21" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="U21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="V21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="W21" s="7" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="V21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="W21" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>6</v>
@@ -3145,19 +3145,19 @@
         <v>6</v>
       </c>
       <c r="Z21" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AA21" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AB21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="AD21" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="AC21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD21" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="AE21" s="3" t="s">
         <v>6</v>
@@ -3166,111 +3166,111 @@
         <v>19</v>
       </c>
       <c r="AG21" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AH21" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>9</v>
+        <v>62</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I22" s="7" t="s">
+      <c r="H22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="P22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P22" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="S22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="T22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="U22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="V22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="W22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="X22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="Z22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE22" s="5" t="s">
-        <v>10</v>
+      <c r="S22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE22" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF22" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AG22" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AH22" s="3" t="s">
         <v>21</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>31</v>
@@ -3371,114 +3371,114 @@
         <v>31</v>
       </c>
       <c r="AF23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AG23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AH23" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>9</v>
+        <v>66</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>9</v>
+      <c r="H24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O24" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P24" s="7" t="s">
+      <c r="O24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="U24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="V24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="W24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="V24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="W24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="X24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AC24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD24" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE24" s="5" t="s">
-        <v>10</v>
+      <c r="AA24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AC24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE24" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="AF24" s="3" t="s">
         <v>24</v>
       </c>
       <c r="AG24" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AH24" s="3" t="s">
         <v>32</v>
@@ -3486,52 +3486,52 @@
     </row>
     <row r="25" ht="18" customHeight="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="L25" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M25" s="3" t="s">
         <v>6</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O25" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="Q25" s="8" t="s">
         <v>31</v>
@@ -3579,13 +3579,13 @@
         <v>31</v>
       </c>
       <c r="AF25" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG25" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AH25" s="3" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" ht="18" customHeight="1" spans="1:100" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rework after review - error messages, calculateMissingFullWeekDays return type
</commit_message>
<xml_diff>
--- a/cypress/fixtures/grafik.xlsx
+++ b/cypress/fixtures/grafik.xlsx
@@ -5,13 +5,14 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="grafik" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="pracownicy" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="75">
   <si>
     <t>GRAFIK</t>
   </si>
@@ -218,13 +219,31 @@
   </si>
   <si>
     <t>Opiekunka 10</t>
+  </si>
+  <si>
+    <t>Imię i nazwisko</t>
+  </si>
+  <si>
+    <t>Stanowisko/funkcja</t>
+  </si>
+  <si>
+    <t>Rodzaj umowy</t>
+  </si>
+  <si>
+    <t>Wymiar czasu pracy</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>UoP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -236,6 +255,9 @@
       <b/>
       <family val="4"/>
       <sz val="28"/>
+    </font>
+    <font>
+      <b/>
     </font>
   </fonts>
   <fills count="8">
@@ -303,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -325,6 +347,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5109,4 +5140,607 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:CV21"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55" defaultColWidth="5"/>
+  <cols>
+    <col min="1" max="1" width="17" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20" style="10" customWidth="1"/>
+    <col min="3" max="3" width="14" style="10" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" t="s">
+        <v>6</v>
+      </c>
+      <c r="W2" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>6</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>6</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>